<commit_message>
dev : players gimanasia
</commit_message>
<xml_diff>
--- a/R/Modulo 2/data/input/Teams.xlsx
+++ b/R/Modulo 2/data/input/Teams.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e.rangel\Documents\emra\Futbol-R-Python-Quarto\R\Modulo 2\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F560A8A-6F1A-405F-BAC7-A159557A9D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11158524-DF10-416A-BFB2-85773CCA2254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="11496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Colombia" sheetId="4" r:id="rId1"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
+    <sheet name="Ecuador" sheetId="5" r:id="rId2"/>
+    <sheet name="Argentina_B" sheetId="6" r:id="rId3"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja3!$A$1:$C$206</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Hoja3!$A$1:$C$206</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="481">
   <si>
     <t>Sevilla</t>
   </si>
@@ -1286,6 +1288,198 @@
   </si>
   <si>
     <t>UMG</t>
+  </si>
+  <si>
+    <t>Delfin</t>
+  </si>
+  <si>
+    <t>Emelec</t>
+  </si>
+  <si>
+    <t>LDU Quito</t>
+  </si>
+  <si>
+    <t>Mushuc Runa</t>
+  </si>
+  <si>
+    <t>Manta</t>
+  </si>
+  <si>
+    <t>Macará</t>
+  </si>
+  <si>
+    <t>Independiente del Valle</t>
+  </si>
+  <si>
+    <t>Deportivo Cuenca</t>
+  </si>
+  <si>
+    <t>El Nacional</t>
+  </si>
+  <si>
+    <t>Aucas</t>
+  </si>
+  <si>
+    <t>Libertad</t>
+  </si>
+  <si>
+    <t>Orense</t>
+  </si>
+  <si>
+    <t>Técnico Universitario</t>
+  </si>
+  <si>
+    <t>Universidad Católica</t>
+  </si>
+  <si>
+    <t>Vinotinto de Ecuador</t>
+  </si>
+  <si>
+    <t>DEL</t>
+  </si>
+  <si>
+    <t>EME</t>
+  </si>
+  <si>
+    <t>LDU</t>
+  </si>
+  <si>
+    <t>MUS</t>
+  </si>
+  <si>
+    <t>MAN</t>
+  </si>
+  <si>
+    <t>MAC</t>
+  </si>
+  <si>
+    <t>INV</t>
+  </si>
+  <si>
+    <t>DEC</t>
+  </si>
+  <si>
+    <t>ENA</t>
+  </si>
+  <si>
+    <t>AUC</t>
+  </si>
+  <si>
+    <t>LIB</t>
+  </si>
+  <si>
+    <t>ORE</t>
+  </si>
+  <si>
+    <t>TUN</t>
+  </si>
+  <si>
+    <t>UNC</t>
+  </si>
+  <si>
+    <t>VIE</t>
+  </si>
+  <si>
+    <t>Chaco For Ever</t>
+  </si>
+  <si>
+    <t>Central Norte</t>
+  </si>
+  <si>
+    <t>Defensores Unidos</t>
+  </si>
+  <si>
+    <t>Temperley</t>
+  </si>
+  <si>
+    <t>Nueva Chicago</t>
+  </si>
+  <si>
+    <t>Agropecuario</t>
+  </si>
+  <si>
+    <t>Club Atlético Mitre</t>
+  </si>
+  <si>
+    <t>Colón</t>
+  </si>
+  <si>
+    <t>Defensores de Belgrano</t>
+  </si>
+  <si>
+    <t>Chacarita Juniors</t>
+  </si>
+  <si>
+    <t>Gimnasia Jujuy</t>
+  </si>
+  <si>
+    <t>Estudiantes Río Cuarto</t>
+  </si>
+  <si>
+    <t>Almirante Brown</t>
+  </si>
+  <si>
+    <t>Talleres Remedios</t>
+  </si>
+  <si>
+    <t>Deportivo Morón</t>
+  </si>
+  <si>
+    <t>Estudiantes Caseros</t>
+  </si>
+  <si>
+    <t>Gimnasia Mendoza</t>
+  </si>
+  <si>
+    <t>San Telmo</t>
+  </si>
+  <si>
+    <t>Agentina</t>
+  </si>
+  <si>
+    <t>GIM</t>
+  </si>
+  <si>
+    <t>CHA</t>
+  </si>
+  <si>
+    <t>EST</t>
+  </si>
+  <si>
+    <t>TAL</t>
+  </si>
+  <si>
+    <t>CFO</t>
+  </si>
+  <si>
+    <t>TEM</t>
+  </si>
+  <si>
+    <t>AGR</t>
+  </si>
+  <si>
+    <t>DEF</t>
+  </si>
+  <si>
+    <t>MIT</t>
+  </si>
+  <si>
+    <t>NUC</t>
+  </si>
+  <si>
+    <t>STE</t>
+  </si>
+  <si>
+    <t>CEN</t>
+  </si>
+  <si>
+    <t>DEU</t>
+  </si>
+  <si>
+    <t>AAE</t>
+  </si>
+  <si>
+    <t>DMO</t>
   </si>
 </sst>
 </file>
@@ -1629,16 +1823,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06546E92-6BDD-4047-B17D-F3F39FBF1647}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>407</v>
       </c>
@@ -1649,7 +1843,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>298</v>
       </c>
@@ -1660,7 +1854,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>299</v>
       </c>
@@ -1671,7 +1865,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>300</v>
       </c>
@@ -1682,7 +1876,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>301</v>
       </c>
@@ -1693,7 +1887,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>302</v>
       </c>
@@ -1704,7 +1898,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>303</v>
       </c>
@@ -1715,7 +1909,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>304</v>
       </c>
@@ -1726,7 +1920,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>305</v>
       </c>
@@ -1737,7 +1931,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>306</v>
       </c>
@@ -1748,7 +1942,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>307</v>
       </c>
@@ -1759,7 +1953,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>308</v>
       </c>
@@ -1770,7 +1964,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>309</v>
       </c>
@@ -1781,7 +1975,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>310</v>
       </c>
@@ -1792,7 +1986,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>311</v>
       </c>
@@ -1803,7 +1997,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>312</v>
       </c>
@@ -1814,7 +2008,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>313</v>
       </c>
@@ -1825,7 +2019,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>314</v>
       </c>
@@ -1836,7 +2030,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>315</v>
       </c>
@@ -1847,7 +2041,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>316</v>
       </c>
@@ -1858,7 +2052,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>317</v>
       </c>
@@ -1869,7 +2063,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>318</v>
       </c>
@@ -1880,7 +2074,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>408</v>
       </c>
@@ -1891,7 +2085,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>409</v>
       </c>
@@ -1902,7 +2096,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>410</v>
       </c>
@@ -1913,7 +2107,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>411</v>
       </c>
@@ -1924,7 +2118,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>412</v>
       </c>
@@ -1941,21 +2135,452 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F10068-7DD3-4107-A771-A585CB6E21E2}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>417</v>
+      </c>
+      <c r="B2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>418</v>
+      </c>
+      <c r="B3" t="s">
+        <v>347</v>
+      </c>
+      <c r="C3" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>419</v>
+      </c>
+      <c r="B4" t="s">
+        <v>347</v>
+      </c>
+      <c r="C4" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>420</v>
+      </c>
+      <c r="B5" t="s">
+        <v>347</v>
+      </c>
+      <c r="C5" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>421</v>
+      </c>
+      <c r="B6" t="s">
+        <v>347</v>
+      </c>
+      <c r="C6" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>422</v>
+      </c>
+      <c r="B7" t="s">
+        <v>347</v>
+      </c>
+      <c r="C7" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>423</v>
+      </c>
+      <c r="B8" t="s">
+        <v>347</v>
+      </c>
+      <c r="C8" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>424</v>
+      </c>
+      <c r="B9" t="s">
+        <v>347</v>
+      </c>
+      <c r="C9" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>425</v>
+      </c>
+      <c r="B10" t="s">
+        <v>347</v>
+      </c>
+      <c r="C10" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>426</v>
+      </c>
+      <c r="B11" t="s">
+        <v>347</v>
+      </c>
+      <c r="C11" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>347</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>427</v>
+      </c>
+      <c r="B13" t="s">
+        <v>347</v>
+      </c>
+      <c r="C13" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>428</v>
+      </c>
+      <c r="B14" t="s">
+        <v>347</v>
+      </c>
+      <c r="C14" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>429</v>
+      </c>
+      <c r="B15" t="s">
+        <v>347</v>
+      </c>
+      <c r="C15" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>430</v>
+      </c>
+      <c r="B16" t="s">
+        <v>347</v>
+      </c>
+      <c r="C16" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>431</v>
+      </c>
+      <c r="B17" t="s">
+        <v>347</v>
+      </c>
+      <c r="C17" t="s">
+        <v>446</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF59FF7-DEE2-40D1-9227-A296856DFEA3}">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>447</v>
+      </c>
+      <c r="B2" t="s">
+        <v>465</v>
+      </c>
+      <c r="C2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>448</v>
+      </c>
+      <c r="B3" t="s">
+        <v>465</v>
+      </c>
+      <c r="C3" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>449</v>
+      </c>
+      <c r="B4" t="s">
+        <v>465</v>
+      </c>
+      <c r="C4" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>450</v>
+      </c>
+      <c r="B5" t="s">
+        <v>465</v>
+      </c>
+      <c r="C5" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>451</v>
+      </c>
+      <c r="B6" t="s">
+        <v>465</v>
+      </c>
+      <c r="C6" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>452</v>
+      </c>
+      <c r="B7" t="s">
+        <v>465</v>
+      </c>
+      <c r="C7" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>453</v>
+      </c>
+      <c r="B8" t="s">
+        <v>465</v>
+      </c>
+      <c r="C8" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>454</v>
+      </c>
+      <c r="B9" t="s">
+        <v>465</v>
+      </c>
+      <c r="C9" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>455</v>
+      </c>
+      <c r="B10" t="s">
+        <v>465</v>
+      </c>
+      <c r="C10" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>456</v>
+      </c>
+      <c r="B11" t="s">
+        <v>465</v>
+      </c>
+      <c r="C11" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>457</v>
+      </c>
+      <c r="B12" t="s">
+        <v>465</v>
+      </c>
+      <c r="C12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>458</v>
+      </c>
+      <c r="B13" t="s">
+        <v>465</v>
+      </c>
+      <c r="C13" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>459</v>
+      </c>
+      <c r="B14" t="s">
+        <v>465</v>
+      </c>
+      <c r="C14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>460</v>
+      </c>
+      <c r="B15" t="s">
+        <v>465</v>
+      </c>
+      <c r="C15" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>461</v>
+      </c>
+      <c r="B16" t="s">
+        <v>465</v>
+      </c>
+      <c r="C16" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>462</v>
+      </c>
+      <c r="B17" t="s">
+        <v>465</v>
+      </c>
+      <c r="C17" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>463</v>
+      </c>
+      <c r="B18" t="s">
+        <v>465</v>
+      </c>
+      <c r="C18" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>464</v>
+      </c>
+      <c r="B19" t="s">
+        <v>465</v>
+      </c>
+      <c r="C19" t="s">
+        <v>476</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:C206"/>
   <sheetViews>
-    <sheetView topLeftCell="A150" workbookViewId="0">
-      <selection sqref="A1:C169"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>407</v>
       </c>
@@ -1966,7 +2591,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1977,7 +2602,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -1988,7 +2613,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1999,7 +2624,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>184</v>
       </c>
@@ -2010,7 +2635,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -2021,7 +2646,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>228</v>
       </c>
@@ -2032,7 +2657,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -2043,7 +2668,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -2054,7 +2679,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -2065,7 +2690,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>229</v>
       </c>
@@ -2076,7 +2701,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>224</v>
       </c>
@@ -2087,7 +2712,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>293</v>
       </c>
@@ -2098,7 +2723,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>185</v>
       </c>
@@ -2109,7 +2734,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -2120,7 +2745,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -2131,7 +2756,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -2142,7 +2767,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>223</v>
       </c>
@@ -2153,7 +2778,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -2164,7 +2789,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>186</v>
       </c>
@@ -2175,7 +2800,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>221</v>
       </c>
@@ -2186,7 +2811,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -2197,7 +2822,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -2208,7 +2833,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>226</v>
       </c>
@@ -2219,7 +2844,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>222</v>
       </c>
@@ -2230,7 +2855,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>225</v>
       </c>
@@ -2241,7 +2866,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>187</v>
       </c>
@@ -2252,7 +2877,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -2263,7 +2888,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>227</v>
       </c>
@@ -2274,7 +2899,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>188</v>
       </c>
@@ -2285,7 +2910,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -2296,7 +2921,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>143</v>
       </c>
@@ -2307,7 +2932,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>133</v>
       </c>
@@ -2318,7 +2943,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>189</v>
       </c>
@@ -2329,7 +2954,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>138</v>
       </c>
@@ -2340,7 +2965,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>249</v>
       </c>
@@ -2351,7 +2976,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>145</v>
       </c>
@@ -2362,7 +2987,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>245</v>
       </c>
@@ -2373,7 +2998,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>247</v>
       </c>
@@ -2384,7 +3009,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>253</v>
       </c>
@@ -2395,7 +3020,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>246</v>
       </c>
@@ -2406,7 +3031,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>137</v>
       </c>
@@ -2417,7 +3042,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>250</v>
       </c>
@@ -2428,7 +3053,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>190</v>
       </c>
@@ -2439,7 +3064,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>191</v>
       </c>
@@ -2450,7 +3075,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>140</v>
       </c>
@@ -2461,7 +3086,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>144</v>
       </c>
@@ -2472,7 +3097,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>139</v>
       </c>
@@ -2483,7 +3108,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>251</v>
       </c>
@@ -2494,7 +3119,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>135</v>
       </c>
@@ -2505,7 +3130,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>192</v>
       </c>
@@ -2516,7 +3141,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>193</v>
       </c>
@@ -2527,7 +3152,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>194</v>
       </c>
@@ -2538,7 +3163,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>134</v>
       </c>
@@ -2549,7 +3174,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>132</v>
       </c>
@@ -2560,7 +3185,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>141</v>
       </c>
@@ -2571,7 +3196,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>252</v>
       </c>
@@ -2582,7 +3207,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>142</v>
       </c>
@@ -2593,7 +3218,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>136</v>
       </c>
@@ -2604,7 +3229,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>248</v>
       </c>
@@ -2615,7 +3240,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>294</v>
       </c>
@@ -2626,7 +3251,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>172</v>
       </c>
@@ -2637,7 +3262,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>173</v>
       </c>
@@ -2648,7 +3273,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>174</v>
       </c>
@@ -2659,7 +3284,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>72</v>
       </c>
@@ -2670,7 +3295,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>175</v>
       </c>
@@ -2681,7 +3306,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>234</v>
       </c>
@@ -2692,7 +3317,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>73</v>
       </c>
@@ -2703,7 +3328,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>176</v>
       </c>
@@ -2714,7 +3339,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>177</v>
       </c>
@@ -2725,7 +3350,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>178</v>
       </c>
@@ -2736,7 +3361,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>230</v>
       </c>
@@ -2747,7 +3372,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>232</v>
       </c>
@@ -2758,7 +3383,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>76</v>
       </c>
@@ -2769,7 +3394,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>179</v>
       </c>
@@ -2780,7 +3405,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>233</v>
       </c>
@@ -2791,7 +3416,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -2802,7 +3427,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>235</v>
       </c>
@@ -2813,7 +3438,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>180</v>
       </c>
@@ -2824,7 +3449,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>181</v>
       </c>
@@ -2835,7 +3460,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>74</v>
       </c>
@@ -2846,7 +3471,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>182</v>
       </c>
@@ -2857,7 +3482,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>231</v>
       </c>
@@ -2868,7 +3493,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>75</v>
       </c>
@@ -2879,7 +3504,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>183</v>
       </c>
@@ -2890,7 +3515,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>195</v>
       </c>
@@ -2901,7 +3526,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>102</v>
       </c>
@@ -2912,7 +3537,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>243</v>
       </c>
@@ -2923,7 +3548,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>196</v>
       </c>
@@ -2934,7 +3559,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>103</v>
       </c>
@@ -2945,7 +3570,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>107</v>
       </c>
@@ -2956,7 +3581,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>238</v>
       </c>
@@ -2967,7 +3592,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>236</v>
       </c>
@@ -2978,7 +3603,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>244</v>
       </c>
@@ -2989,7 +3614,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>240</v>
       </c>
@@ -3000,7 +3625,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>241</v>
       </c>
@@ -3011,7 +3636,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>106</v>
       </c>
@@ -3022,7 +3647,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>239</v>
       </c>
@@ -3033,7 +3658,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -3044,7 +3669,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>197</v>
       </c>
@@ -3055,7 +3680,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>95</v>
       </c>
@@ -3066,7 +3691,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>97</v>
       </c>
@@ -3077,7 +3702,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>108</v>
       </c>
@@ -3088,7 +3713,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>198</v>
       </c>
@@ -3099,7 +3724,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>237</v>
       </c>
@@ -3110,7 +3735,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>101</v>
       </c>
@@ -3121,7 +3746,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>199</v>
       </c>
@@ -3132,7 +3757,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>242</v>
       </c>
@@ -3143,7 +3768,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>105</v>
       </c>
@@ -3154,7 +3779,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -3165,7 +3790,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>100</v>
       </c>
@@ -3176,7 +3801,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>200</v>
       </c>
@@ -3187,7 +3812,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>291</v>
       </c>
@@ -3198,7 +3823,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>96</v>
       </c>
@@ -3209,7 +3834,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>104</v>
       </c>
@@ -3220,7 +3845,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>99</v>
       </c>
@@ -3231,7 +3856,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>165</v>
       </c>
@@ -3242,7 +3867,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>207</v>
       </c>
@@ -3253,7 +3878,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>166</v>
       </c>
@@ -3264,7 +3889,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>167</v>
       </c>
@@ -3275,7 +3900,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>4</v>
       </c>
@@ -3286,7 +3911,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>287</v>
       </c>
@@ -3297,7 +3922,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>168</v>
       </c>
@@ -3308,7 +3933,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>213</v>
       </c>
@@ -3319,7 +3944,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>209</v>
       </c>
@@ -3330,7 +3955,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>10</v>
       </c>
@@ -3341,7 +3966,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>212</v>
       </c>
@@ -3352,7 +3977,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>11</v>
       </c>
@@ -3363,7 +3988,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>9</v>
       </c>
@@ -3374,7 +3999,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>202</v>
       </c>
@@ -3385,7 +4010,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>5</v>
       </c>
@@ -3396,7 +4021,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>210</v>
       </c>
@@ -3407,7 +4032,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>169</v>
       </c>
@@ -3418,7 +4043,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>1</v>
       </c>
@@ -3429,7 +4054,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>211</v>
       </c>
@@ -3440,7 +4065,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>7</v>
       </c>
@@ -3451,7 +4076,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>3</v>
       </c>
@@ -3462,7 +4087,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>201</v>
       </c>
@@ -3473,7 +4098,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>170</v>
       </c>
@@ -3484,7 +4109,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>2</v>
       </c>
@@ -3495,7 +4120,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>14</v>
       </c>
@@ -3506,7 +4131,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>171</v>
       </c>
@@ -3517,7 +4142,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>206</v>
       </c>
@@ -3528,7 +4153,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>0</v>
       </c>
@@ -3539,7 +4164,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>208</v>
       </c>
@@ -3550,7 +4175,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>6</v>
       </c>
@@ -3561,7 +4186,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>8</v>
       </c>
@@ -3572,7 +4197,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>295</v>
       </c>
@@ -3583,7 +4208,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>298</v>
       </c>
@@ -3594,7 +4219,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>299</v>
       </c>
@@ -3605,7 +4230,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>300</v>
       </c>
@@ -3616,7 +4241,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>301</v>
       </c>
@@ -3627,7 +4252,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>302</v>
       </c>
@@ -3638,7 +4263,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>303</v>
       </c>
@@ -3649,7 +4274,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>304</v>
       </c>
@@ -3660,7 +4285,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>305</v>
       </c>
@@ -3671,7 +4296,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>306</v>
       </c>
@@ -3682,7 +4307,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>307</v>
       </c>
@@ -3693,7 +4318,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>308</v>
       </c>
@@ -3704,7 +4329,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>309</v>
       </c>
@@ -3715,7 +4340,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>310</v>
       </c>
@@ -3726,7 +4351,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>311</v>
       </c>
@@ -3737,7 +4362,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>312</v>
       </c>
@@ -3748,7 +4373,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>313</v>
       </c>
@@ -3759,7 +4384,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>314</v>
       </c>
@@ -3770,7 +4395,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>315</v>
       </c>
@@ -3781,7 +4406,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>316</v>
       </c>
@@ -3792,7 +4417,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>317</v>
       </c>
@@ -3803,7 +4428,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>318</v>
       </c>
@@ -3814,7 +4439,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>354</v>
       </c>
@@ -3825,7 +4450,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>347</v>
       </c>
@@ -3836,7 +4461,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>349</v>
       </c>
@@ -3847,7 +4472,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>348</v>
       </c>
@@ -3858,7 +4483,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>297</v>
       </c>
@@ -3869,7 +4494,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>355</v>
       </c>
@@ -3880,7 +4505,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>350</v>
       </c>
@@ -3891,7 +4516,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>351</v>
       </c>
@@ -3902,7 +4527,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>352</v>
       </c>
@@ -3913,7 +4538,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>353</v>
       </c>
@@ -3924,7 +4549,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>393</v>
       </c>
@@ -3935,7 +4560,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>358</v>
       </c>
@@ -3946,7 +4571,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>388</v>
       </c>
@@ -3957,7 +4582,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>359</v>
       </c>
@@ -3968,7 +4593,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>394</v>
       </c>
@@ -3979,7 +4604,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>360</v>
       </c>
@@ -3990,7 +4615,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>361</v>
       </c>
@@ -4001,7 +4626,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="187" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>395</v>
       </c>
@@ -4012,7 +4637,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>396</v>
       </c>
@@ -4023,7 +4648,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>362</v>
       </c>
@@ -4034,7 +4659,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>390</v>
       </c>
@@ -4045,7 +4670,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>389</v>
       </c>
@@ -4056,7 +4681,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>397</v>
       </c>
@@ -4067,7 +4692,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>398</v>
       </c>
@@ -4078,7 +4703,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>399</v>
       </c>
@@ -4089,7 +4714,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>386</v>
       </c>
@@ -4100,7 +4725,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>400</v>
       </c>
@@ -4111,7 +4736,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>401</v>
       </c>
@@ -4122,7 +4747,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>363</v>
       </c>
@@ -4133,7 +4758,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>402</v>
       </c>
@@ -4144,7 +4769,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>364</v>
       </c>
@@ -4155,7 +4780,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>356</v>
       </c>
@@ -4166,7 +4791,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>403</v>
       </c>
@@ -4177,7 +4802,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>406</v>
       </c>
@@ -4188,7 +4813,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>387</v>
       </c>
@@ -4199,7 +4824,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="205" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>404</v>
       </c>
@@ -4210,7 +4835,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>405</v>
       </c>
@@ -4222,13 +4847,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C206" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Colombia"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C206" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A180:D206">
     <sortCondition ref="C180:C206"/>
   </sortState>

</xml_diff>